<commit_message>
Huge CSS Revamp, added first test checking all grids
</commit_message>
<xml_diff>
--- a/Execon_-_TMO_SML_TS01.xlsx
+++ b/Execon_-_TMO_SML_TS01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\TMO.R.AutomatedTestsSML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13F159F-FD94-4271-94C4-EB8FAE616FEB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56A0CED-12B2-4077-A11F-98B1C018219E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16665" windowHeight="5130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
     <t>TC01</t>
   </si>
   <si>
-    <t>nie</t>
+    <t>tak</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B3" sqref="B3:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>